<commit_message>
update folder structure, log of the project
</commit_message>
<xml_diff>
--- a/LOG.xlsx
+++ b/LOG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="581"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" tabRatio="581"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Timestamp</t>
   </si>
@@ -102,28 +102,61 @@
     <t>Test pretrained 1119-224829_svm on 3 testing regions</t>
   </si>
   <si>
-    <t xml:space="preserve">Try different normalization and imputation methods for preparing data </t>
-  </si>
-  <si>
     <t>evaluate by metrics, open datasets, feature importance. All test regions show good results (Acc &gt;=0.8)</t>
   </si>
   <si>
-    <t>normalization = {None, normalize, standardize, divide bands by 10000}; imputation = {fill 0, forward filling, linear interpolation}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check computational cost </t>
-  </si>
-  <si>
-    <t xml:space="preserve">computational cost to train three models and to infer further data </t>
-  </si>
-  <si>
     <t>Handle spatial autocorrelation</t>
   </si>
   <si>
-    <t>Un/semi-supervised learning for apples classification</t>
-  </si>
-  <si>
-    <t>Three models (OCSVM, PUL, PUL-w)</t>
+    <t>normalization = {float, reflectance, normalize, standardize}; imputation = {fill 0, forward filling, linear interpolation}</t>
+  </si>
+  <si>
+    <t>cropland_1206-215716.log -- cropland_1212-232444.log</t>
+  </si>
+  <si>
+    <t>fa718209df583a9c48b2c825f25b310ef0468816</t>
+  </si>
+  <si>
+    <t>Try different normalization and imputation methods</t>
+  </si>
+  <si>
+    <t>54d2e4be4fbad9f623166c0f80e8b565da3df7ab</t>
+  </si>
+  <si>
+    <t>cropland_20220104-112305.log</t>
+  </si>
+  <si>
+    <t>Change cloud mask</t>
+  </si>
+  <si>
+    <t>use scene classification results from Sen2Cor rather than the built-in mask</t>
+  </si>
+  <si>
+    <t>Feature selection</t>
+  </si>
+  <si>
+    <t>run feature selection for rfc: {temporal, temporal+ndvi_spatial, temporal+spatial, select}</t>
+  </si>
+  <si>
+    <t>cropland_20220105-135132.log -- cropland_20220111-094108.log</t>
+  </si>
+  <si>
+    <t>139c94e3e54f8999023c00cdd34e4e92552df70b</t>
+  </si>
+  <si>
+    <t>cropland_20220117-172418_predict.log</t>
+  </si>
+  <si>
+    <t>Generate cropland map</t>
+  </si>
+  <si>
+    <t>make cropland predictions on 4 tiles</t>
+  </si>
+  <si>
+    <t>tiles 43SFR, 43RFQ, 43SGR, 43SGR</t>
+  </si>
+  <si>
+    <t>af9bf4de1aa966d1ce515c6a727f2238581c5c7a</t>
   </si>
 </sst>
 </file>
@@ -456,21 +489,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+    <col min="3" max="3" width="44.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="44.85546875" customWidth="1"/>
+    <col min="6" max="6" width="44.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -498,57 +531,87 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>44578</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>44572</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>44565</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>44542</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>44527</v>
       </c>
@@ -565,10 +628,10 @@
         <v>26</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>44524</v>
       </c>
@@ -588,7 +651,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>44492</v>
       </c>
@@ -602,13 +665,13 @@
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>44477</v>
       </c>
@@ -628,7 +691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>44468</v>
       </c>

</xml_diff>